<commit_message>
fixed bugs in crm workflow descriptions
</commit_message>
<xml_diff>
--- a/notebooks/data_loading/equity_fund_example.xlsx
+++ b/notebooks/data_loading/equity_fund_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lilycampbell/Desktop/Capstone_I/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8B475A-C324-9B40-8506-87904F0C498E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74BEF0B3-347B-404B-9CD2-D1FB5AA86A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="900" windowWidth="29080" windowHeight="16840" xr2:uid="{F8CA6F91-01A4-9644-8B8D-C3A773915286}"/>
   </bookViews>
@@ -206,18 +206,6 @@
     <t>fund</t>
   </si>
   <si>
-    <t>ftiex</t>
-  </si>
-  <si>
-    <t>fxaix</t>
-  </si>
-  <si>
-    <t>fcntx</t>
-  </si>
-  <si>
-    <t>vsmpx</t>
-  </si>
-  <si>
     <t>weight</t>
   </si>
   <si>
@@ -261,6 +249,18 @@
   </si>
   <si>
     <t>bond</t>
+  </si>
+  <si>
+    <t>FTIEX</t>
+  </si>
+  <si>
+    <t>FXAIX</t>
+  </si>
+  <si>
+    <t>FCNTX</t>
+  </si>
+  <si>
+    <t>VSMPX</t>
   </si>
 </sst>
 </file>
@@ -643,7 +643,7 @@
   <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -663,10 +663,10 @@
         <v>55</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -677,13 +677,13 @@
         <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D2">
         <v>0.05</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -694,13 +694,13 @@
         <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D3">
         <v>0.2</v>
       </c>
       <c r="E3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -711,13 +711,13 @@
         <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D4">
         <v>0.05</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -728,13 +728,13 @@
         <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D5">
         <v>0.1</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -745,13 +745,13 @@
         <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D6">
         <v>0.1</v>
       </c>
       <c r="E6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -762,13 +762,13 @@
         <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D7">
         <v>0.2</v>
       </c>
       <c r="E7" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -779,13 +779,13 @@
         <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D8">
         <v>0.1</v>
       </c>
       <c r="E8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -796,13 +796,13 @@
         <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D9">
         <v>0.15</v>
       </c>
       <c r="E9" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -813,13 +813,13 @@
         <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D10">
         <v>0.04</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -830,13 +830,13 @@
         <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D11">
         <v>0.01</v>
       </c>
       <c r="E11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -847,13 +847,13 @@
         <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D12">
         <v>0.06</v>
       </c>
       <c r="E12" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -864,13 +864,13 @@
         <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D13">
         <v>0.1</v>
       </c>
       <c r="E13" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -881,13 +881,13 @@
         <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D14">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E14" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -898,13 +898,13 @@
         <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D15">
         <v>0.1</v>
       </c>
       <c r="E15" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -915,13 +915,13 @@
         <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D16">
         <v>0.1</v>
       </c>
       <c r="E16" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -932,13 +932,13 @@
         <v>43</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D17">
         <v>0.04</v>
       </c>
       <c r="E17" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -949,13 +949,13 @@
         <v>44</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D18">
         <v>0.04</v>
       </c>
       <c r="E18" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -966,13 +966,13 @@
         <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D19">
         <v>0.3</v>
       </c>
       <c r="E19" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -983,13 +983,13 @@
         <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D20">
         <v>0.03</v>
       </c>
       <c r="E20" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1000,13 +1000,13 @@
         <v>47</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D21">
         <v>0.16</v>
       </c>
       <c r="E21" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1017,13 +1017,13 @@
         <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D22">
         <v>0.08</v>
       </c>
       <c r="E22" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1034,13 +1034,13 @@
         <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D23">
         <v>0.1</v>
       </c>
       <c r="E23" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1051,13 +1051,13 @@
         <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D24">
         <v>0.25</v>
       </c>
       <c r="E24" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1068,13 +1068,13 @@
         <v>41</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D25">
         <v>0.14000000000000001</v>
       </c>
       <c r="E25" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1085,13 +1085,13 @@
         <v>42</v>
       </c>
       <c r="C26" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D26">
         <v>0.16</v>
       </c>
       <c r="E26" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1102,13 +1102,13 @@
         <v>43</v>
       </c>
       <c r="C27" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D27">
         <v>0.06</v>
       </c>
       <c r="E27" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1119,13 +1119,13 @@
         <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D28">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E28" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1136,13 +1136,13 @@
         <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D29">
         <v>0.03</v>
       </c>
       <c r="E29" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1153,13 +1153,13 @@
         <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D30">
         <v>0.1</v>
       </c>
       <c r="E30" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -1170,13 +1170,13 @@
         <v>53</v>
       </c>
       <c r="C31" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D31">
         <v>0.01</v>
       </c>
       <c r="E31" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1187,13 +1187,13 @@
         <v>38</v>
       </c>
       <c r="C32" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="D32">
         <v>0.18</v>
       </c>
       <c r="E32" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -1204,13 +1204,13 @@
         <v>39</v>
       </c>
       <c r="C33" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="D33">
         <v>0.06</v>
       </c>
       <c r="E33" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1221,13 +1221,13 @@
         <v>40</v>
       </c>
       <c r="C34" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="D34">
         <v>0.09</v>
       </c>
       <c r="E34" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1238,13 +1238,13 @@
         <v>41</v>
       </c>
       <c r="C35" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="D35">
         <v>0.05</v>
       </c>
       <c r="E35" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1255,13 +1255,13 @@
         <v>51</v>
       </c>
       <c r="C36" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="D36">
         <v>0.01</v>
       </c>
       <c r="E36" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1272,13 +1272,13 @@
         <v>52</v>
       </c>
       <c r="C37" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="D37">
         <v>0.13</v>
       </c>
       <c r="E37" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1289,13 +1289,13 @@
         <v>53</v>
       </c>
       <c r="C38" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="D38">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E38" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -1306,13 +1306,13 @@
         <v>45</v>
       </c>
       <c r="C39" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="D39">
         <v>0.12</v>
       </c>
       <c r="E39" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -1323,13 +1323,13 @@
         <v>46</v>
       </c>
       <c r="C40" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="D40">
         <v>0.15</v>
       </c>
       <c r="E40" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -1340,268 +1340,268 @@
         <v>47</v>
       </c>
       <c r="C41" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="D41">
         <v>0.14000000000000001</v>
       </c>
       <c r="E41" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B42" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C42" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D42">
         <v>0.3</v>
       </c>
       <c r="E42" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B43" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C43" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D43">
         <v>0.3</v>
       </c>
       <c r="E43" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B44" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C44" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D44">
         <v>0.4</v>
       </c>
       <c r="E44" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B45" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C45" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D45">
         <v>0.2</v>
       </c>
       <c r="E45" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46" t="s">
+        <v>61</v>
+      </c>
+      <c r="C46" t="s">
         <v>64</v>
-      </c>
-      <c r="B46" t="s">
-        <v>65</v>
-      </c>
-      <c r="C46" t="s">
-        <v>68</v>
       </c>
       <c r="D46">
         <v>0.4</v>
       </c>
       <c r="E46" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B47" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C47" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D47">
         <v>0.4</v>
       </c>
       <c r="E47" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B48" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C48" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D48">
         <v>0.2</v>
       </c>
       <c r="E48" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B49" t="s">
+        <v>61</v>
+      </c>
+      <c r="C49" t="s">
         <v>65</v>
-      </c>
-      <c r="C49" t="s">
-        <v>69</v>
       </c>
       <c r="D49">
         <v>0.2</v>
       </c>
       <c r="E49" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B50" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C50" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D50">
         <v>0.6</v>
       </c>
       <c r="E50" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B51" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C51" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D51">
         <v>0.5</v>
       </c>
       <c r="E51" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B52" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C52" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D52">
         <v>0.2</v>
       </c>
       <c r="E52" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>62</v>
+      </c>
+      <c r="B53" t="s">
+        <v>63</v>
+      </c>
+      <c r="C53" t="s">
         <v>66</v>
-      </c>
-      <c r="B53" t="s">
-        <v>67</v>
-      </c>
-      <c r="C53" t="s">
-        <v>70</v>
       </c>
       <c r="D53">
         <v>0.3</v>
       </c>
       <c r="E53" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B54" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C54" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D54">
         <v>0.1</v>
       </c>
       <c r="E54" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B55" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C55" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D55">
         <v>0.2</v>
       </c>
       <c r="E55" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B56" t="s">
+        <v>63</v>
+      </c>
+      <c r="C56" t="s">
         <v>67</v>
-      </c>
-      <c r="C56" t="s">
-        <v>71</v>
       </c>
       <c r="D56">
         <v>0.7</v>
       </c>
       <c r="E56" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>